<commit_message>
Add revenue data for "water & waste" industry (water treatment, wastewater, solid waste collection, landfilling, recycling, etc.)
</commit_message>
<xml_diff>
--- a/InputData/indst/TNRbI/Total Nonfuel Revenue by Industry.xlsx
+++ b/InputData/indst/TNRbI/Total Nonfuel Revenue by Industry.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\indst\TNRbI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\indst\TNRbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E73BBC-694A-40FD-A4E4-D8EF4998CCA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="25875" windowHeight="12600"/>
+    <workbookView xWindow="2985" yWindow="2250" windowWidth="24765" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="EIA 24" sheetId="4" r:id="rId2"/>
-    <sheet name="TNRbI" sheetId="3" r:id="rId3"/>
+    <sheet name="water &amp; waste" sheetId="5" r:id="rId3"/>
+    <sheet name="TNRbI" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="currency_conv">About!$A$49</definedName>
+    <definedName name="currency_conv">About!$A$65</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="174">
   <si>
     <t>Source:</t>
   </si>
@@ -399,21 +411,6 @@
   </si>
   <si>
     <t>2012 USD / billion 2009 USD</t>
-  </si>
-  <si>
-    <t>The "waste management" industry in the EPS doesn't have</t>
-  </si>
-  <si>
-    <t>data in EIA AEO, and water treatment (the largest part of that industry)</t>
-  </si>
-  <si>
-    <t>is often government-run or a regulated monopoly that is not</t>
-  </si>
-  <si>
-    <t>profit-driven, so we do not attempt to calculate revenue changes</t>
-  </si>
-  <si>
-    <t>for the waste management industry.</t>
   </si>
   <si>
     <t>Currency conversion</t>
@@ -487,15 +484,112 @@
     <t>TNRbI Total Nonfuel Revenue by Industry</t>
   </si>
   <si>
-    <t>Nonfuel Revenue ($)</t>
+    <t>Water Industry Revenues</t>
+  </si>
+  <si>
+    <t>The water industry includes drinking water treatment, water distribution, and wastewater/sewer services and treatment.</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>billion 2018 USD</t>
+  </si>
+  <si>
+    <t>Solid Waste Management Revenues</t>
+  </si>
+  <si>
+    <t>Water treatment, distribution, sewer / wastewater treatment</t>
+  </si>
+  <si>
+    <t>Environmental Buisness News</t>
+  </si>
+  <si>
+    <t>U.S. Water Industry grows to $172 billion; 4% growth forecast for 2018</t>
+  </si>
+  <si>
+    <t>https://ebionline.org/2018/10/03/u-s-water-industry-grows-to-172-billion-4-growth-forecast-for-2018/</t>
+  </si>
+  <si>
+    <t>Paragraph 2</t>
+  </si>
+  <si>
+    <t>Solid waste collection, landfilling, recycling, composting</t>
+  </si>
+  <si>
+    <t>The solid waste industry includes solid waste collection, landfilling, recycling, composting, etc.</t>
+  </si>
+  <si>
+    <t>Public companies increased control of $74B US waste industry in 2018</t>
+  </si>
+  <si>
+    <t>WasteDive</t>
+  </si>
+  <si>
+    <t>https://www.wastedive.com/news/public-companies-increased-control-of-74b-us-waste-industry-in-2018/556079/</t>
+  </si>
+  <si>
+    <t>Bullet 1</t>
+  </si>
+  <si>
+    <t>Most Non-Energy Industries Industries</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>U.S. Population Projections (for scaling)</t>
+  </si>
+  <si>
+    <t>Solid Waste Industry Revenues</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Population Projections (for scaling water &amp; waste revenue)</t>
+  </si>
+  <si>
+    <t>U.N.</t>
+  </si>
+  <si>
+    <t>World Population Prospects 2019</t>
+  </si>
+  <si>
+    <t>https://population.un.org/wpp/Download/Standard/Population/</t>
+  </si>
+  <si>
+    <t>Total population, Medium case (and historical values for years before 2020)</t>
+  </si>
+  <si>
+    <t>2012 USD / 2017 USD</t>
+  </si>
+  <si>
+    <t>2012 USD / 2018 USD</t>
+  </si>
+  <si>
+    <t>billion 2012 USD</t>
+  </si>
+  <si>
+    <t>Nonfuel Revenue (2012 USD)</t>
+  </si>
+  <si>
+    <t>Water &amp; Waste Revenues (billion 2012 USD)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -565,7 +659,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +675,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,7 +757,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -718,17 +824,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="7"/>
-    <cellStyle name="Footnotes: top row" xfId="3"/>
-    <cellStyle name="Header: bottom row" xfId="6"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Parent row" xfId="4"/>
-    <cellStyle name="Table title" xfId="8"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Table title" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -819,6 +933,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -854,6 +985,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1029,235 +1177,327 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" s="26">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="26">
         <f>1.07*10^9</f>
         <v>1070000000.0000001</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B65" t="s">
         <v>124</v>
       </c>
     </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0.93665959530026111</v>
+      </c>
+      <c r="B67" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0.9143273584567535</v>
+      </c>
+      <c r="B68" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{C2BAA05B-6AB9-4540-B9F9-5D773918ABDB}"/>
+    <hyperlink ref="B21" r:id="rId2" xr:uid="{606512E4-D159-461C-8BCF-26B7306F3F80}"/>
+    <hyperlink ref="B28" r:id="rId3" xr:uid="{043A74D7-0FD2-477E-AEC4-A9319F8D9F68}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1267,14 +1507,14 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.86328125" style="4" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.73046875" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="4"/>
+    <col min="1" max="1" width="20.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>107</v>
       </c>
@@ -1381,8 +1621,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="17" t="s">
         <v>106</v>
       </c>
@@ -1393,7 +1633,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="17" t="s">
         <v>104</v>
       </c>
@@ -1406,7 +1646,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="17" t="s">
         <v>101</v>
       </c>
@@ -1417,7 +1657,7 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="17" t="s">
         <v>99</v>
       </c>
@@ -1428,7 +1668,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>97</v>
       </c>
@@ -1436,12 +1676,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15" t="s">
         <v>2</v>
       </c>
@@ -1551,7 +1791,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>94</v>
       </c>
@@ -1661,8 +1901,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>93</v>
       </c>
@@ -1775,7 +2015,7 @@
         <v>1.8898000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>91</v>
       </c>
@@ -1888,17 +2128,17 @@
         <v>5.8120000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>87</v>
       </c>
@@ -2011,7 +2251,7 @@
         <v>1.1761000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>85</v>
       </c>
@@ -2124,7 +2364,7 @@
         <v>1.107E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>84</v>
       </c>
@@ -2237,12 +2477,12 @@
         <v>1.4662E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>82</v>
       </c>
@@ -2355,7 +2595,7 @@
         <v>1.7756000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>80</v>
       </c>
@@ -2468,7 +2708,7 @@
         <v>6.1960000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>78</v>
       </c>
@@ -2581,7 +2821,7 @@
         <v>-1.7729999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>76</v>
       </c>
@@ -2694,7 +2934,7 @@
         <v>1.0227999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>74</v>
       </c>
@@ -2807,7 +3047,7 @@
         <v>1.4657999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>72</v>
       </c>
@@ -2920,7 +3160,7 @@
         <v>9.9909999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>70</v>
       </c>
@@ -3033,7 +3273,7 @@
         <v>1.7110000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>68</v>
       </c>
@@ -3146,7 +3386,7 @@
         <v>1.9053E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>66</v>
       </c>
@@ -3259,7 +3499,7 @@
         <v>1.5769999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>64</v>
       </c>
@@ -3372,7 +3612,7 @@
         <v>-2.7539999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>62</v>
       </c>
@@ -3485,7 +3725,7 @@
         <v>1.9487000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>60</v>
       </c>
@@ -3598,7 +3838,7 @@
         <v>1.8273000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>58</v>
       </c>
@@ -3711,7 +3951,7 @@
         <v>5.829E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>56</v>
       </c>
@@ -3824,7 +4064,7 @@
         <v>2.2030000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>54</v>
       </c>
@@ -3937,7 +4177,7 @@
         <v>-2.575E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>52</v>
       </c>
@@ -4050,7 +4290,7 @@
         <v>-2.4510000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>50</v>
       </c>
@@ -4163,7 +4403,7 @@
         <v>-4.176E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>48</v>
       </c>
@@ -4276,7 +4516,7 @@
         <v>2.3494999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>46</v>
       </c>
@@ -4389,7 +4629,7 @@
         <v>1.8002000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>44</v>
       </c>
@@ -4502,7 +4742,7 @@
         <v>1.2220999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>42</v>
       </c>
@@ -4615,7 +4855,7 @@
         <v>1.6796999999999999E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>40</v>
       </c>
@@ -4728,7 +4968,7 @@
         <v>1.9954E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>38</v>
       </c>
@@ -4841,7 +5081,7 @@
         <v>9.5680000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>36</v>
       </c>
@@ -4954,7 +5194,7 @@
         <v>-7.7800000000000005E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>34</v>
       </c>
@@ -5067,7 +5307,7 @@
         <v>8.8459999999999997E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:37" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>32</v>
       </c>
@@ -5180,7 +5420,7 @@
         <v>2.0156E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>30</v>
       </c>
@@ -5293,7 +5533,7 @@
         <v>1.8870000000000001E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>28</v>
       </c>
@@ -5406,7 +5646,7 @@
         <v>2.6143E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>26</v>
       </c>
@@ -5519,7 +5759,7 @@
         <v>2.5361000000000002E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>24</v>
       </c>
@@ -5632,7 +5872,7 @@
         <v>2.5756000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>22</v>
       </c>
@@ -5745,7 +5985,7 @@
         <v>2.6575999999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>20</v>
       </c>
@@ -5858,7 +6098,7 @@
         <v>2.8815E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>18</v>
       </c>
@@ -5971,8 +6211,8 @@
         <v>1.7311E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="29" t="s">
         <v>16</v>
       </c>
@@ -6012,17 +6252,17 @@
       <c r="AJ62" s="29"/>
       <c r="AK62" s="29"/>
     </row>
-    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="5" t="s">
         <v>13</v>
       </c>
@@ -6037,7 +6277,761 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AEF021-D15D-429C-B757-3F06EC4C5831}">
+  <dimension ref="A1:AJ22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B5" s="2">
+        <v>172</v>
+      </c>
+      <c r="C5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B6" s="34">
+        <f>B5/About!A67</f>
+        <v>183.63127956305479</v>
+      </c>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B12" s="2">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B13" s="34">
+        <f>B12/About!A68</f>
+        <v>78.746413233795309</v>
+      </c>
+      <c r="C13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2022</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2024</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2025</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2026</v>
+      </c>
+      <c r="M16" s="1">
+        <v>2027</v>
+      </c>
+      <c r="N16" s="1">
+        <v>2028</v>
+      </c>
+      <c r="O16" s="1">
+        <v>2029</v>
+      </c>
+      <c r="P16" s="1">
+        <v>2030</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>2031</v>
+      </c>
+      <c r="R16" s="1">
+        <v>2032</v>
+      </c>
+      <c r="S16" s="1">
+        <v>2033</v>
+      </c>
+      <c r="T16" s="1">
+        <v>2034</v>
+      </c>
+      <c r="U16" s="1">
+        <v>2035</v>
+      </c>
+      <c r="V16" s="1">
+        <v>2036</v>
+      </c>
+      <c r="W16" s="1">
+        <v>2037</v>
+      </c>
+      <c r="X16" s="1">
+        <v>2038</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>2039</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>2040</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>2041</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>2042</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>2043</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>2044</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AG16" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AH16" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AI16" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AJ16" s="1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="31">
+        <v>323015.99200000003</v>
+      </c>
+      <c r="C17" s="31">
+        <v>325084.75799999997</v>
+      </c>
+      <c r="D17" s="31">
+        <v>327096.26299999998</v>
+      </c>
+      <c r="E17" s="31">
+        <v>329064.91700000002</v>
+      </c>
+      <c r="F17" s="31">
+        <v>331002.647</v>
+      </c>
+      <c r="G17" s="31">
+        <v>332915.07400000002</v>
+      </c>
+      <c r="H17" s="31">
+        <v>334805.26799999998</v>
+      </c>
+      <c r="I17" s="31">
+        <v>336679.23100000003</v>
+      </c>
+      <c r="J17" s="31">
+        <v>338542.56199999998</v>
+      </c>
+      <c r="K17" s="31">
+        <v>340399.60399999999</v>
+      </c>
+      <c r="L17" s="31">
+        <v>342251.97499999998</v>
+      </c>
+      <c r="M17" s="31">
+        <v>344100.69900000002</v>
+      </c>
+      <c r="N17" s="31">
+        <v>345947.84700000001</v>
+      </c>
+      <c r="O17" s="31">
+        <v>347795.04100000003</v>
+      </c>
+      <c r="P17" s="31">
+        <v>349641.87599999999</v>
+      </c>
+      <c r="Q17" s="31">
+        <v>351490.17800000001</v>
+      </c>
+      <c r="R17" s="31">
+        <v>353335.45199999999</v>
+      </c>
+      <c r="S17" s="31">
+        <v>355162.92</v>
+      </c>
+      <c r="T17" s="31">
+        <v>356952.97200000001</v>
+      </c>
+      <c r="U17" s="31">
+        <v>358690.99699999997</v>
+      </c>
+      <c r="V17" s="31">
+        <v>360371.86</v>
+      </c>
+      <c r="W17" s="31">
+        <v>361997.62</v>
+      </c>
+      <c r="X17" s="31">
+        <v>363569.99699999997</v>
+      </c>
+      <c r="Y17" s="31">
+        <v>365093.53600000002</v>
+      </c>
+      <c r="Z17" s="31">
+        <v>366572.15</v>
+      </c>
+      <c r="AA17" s="31">
+        <v>368006.42499999999</v>
+      </c>
+      <c r="AB17" s="31">
+        <v>369396.55499999999</v>
+      </c>
+      <c r="AC17" s="31">
+        <v>370746.30499999999</v>
+      </c>
+      <c r="AD17" s="31">
+        <v>372060.39399999997</v>
+      </c>
+      <c r="AE17" s="31">
+        <v>373343.35700000002</v>
+      </c>
+      <c r="AF17" s="31">
+        <v>374598.06800000003</v>
+      </c>
+      <c r="AG17" s="31">
+        <v>375827.63400000002</v>
+      </c>
+      <c r="AH17" s="31">
+        <v>377037.24400000001</v>
+      </c>
+      <c r="AI17" s="31">
+        <v>378232.679</v>
+      </c>
+      <c r="AJ17" s="31">
+        <v>379419.09700000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="35">
+        <f>B6</f>
+        <v>183.63127956305479</v>
+      </c>
+      <c r="D20" s="32">
+        <f>$C20*(D17/$C17)</f>
+        <v>184.7675224286692</v>
+      </c>
+      <c r="E20" s="32">
+        <f>$C20*(E17/$C17)</f>
+        <v>185.87955996392927</v>
+      </c>
+      <c r="F20" s="32">
+        <f>$C20*(F17/$C17)</f>
+        <v>186.97412939725751</v>
+      </c>
+      <c r="G20" s="32">
+        <f>$C20*(G17/$C17)</f>
+        <v>188.05440587420307</v>
+      </c>
+      <c r="H20" s="32">
+        <f>$C20*(H17/$C17)</f>
+        <v>189.12212355182606</v>
+      </c>
+      <c r="I20" s="32">
+        <f>$C20*(I17/$C17)</f>
+        <v>190.18067279191021</v>
+      </c>
+      <c r="J20" s="32">
+        <f>$C20*(J17/$C17)</f>
+        <v>191.23321631282022</v>
+      </c>
+      <c r="K20" s="32">
+        <f>$C20*(K17/$C17)</f>
+        <v>192.2822073536808</v>
+      </c>
+      <c r="L20" s="32">
+        <f>$C20*(L17/$C17)</f>
+        <v>193.32855987739862</v>
+      </c>
+      <c r="M20" s="32">
+        <f>$C20*(M17/$C17)</f>
+        <v>194.37285231290846</v>
+      </c>
+      <c r="N20" s="32">
+        <f>$C20*(N17/$C17)</f>
+        <v>195.41625451013584</v>
+      </c>
+      <c r="O20" s="32">
+        <f>$C20*(O17/$C17)</f>
+        <v>196.45968269147554</v>
+      </c>
+      <c r="P20" s="32">
+        <f>$C20*(P17/$C17)</f>
+        <v>197.50290808376488</v>
+      </c>
+      <c r="Q20" s="32">
+        <f>$C20*(Q17/$C17)</f>
+        <v>198.54696214328786</v>
+      </c>
+      <c r="R20" s="32">
+        <f>$C20*(R17/$C17)</f>
+        <v>199.58930577037489</v>
+      </c>
+      <c r="S20" s="32">
+        <f>$C20*(S17/$C17)</f>
+        <v>200.62159128651263</v>
+      </c>
+      <c r="T20" s="32">
+        <f>$C20*(T17/$C17)</f>
+        <v>201.6327415516518</v>
+      </c>
+      <c r="U20" s="32">
+        <f>$C20*(U17/$C17)</f>
+        <v>202.61450322090414</v>
+      </c>
+      <c r="V20" s="32">
+        <f>$C20*(V17/$C17)</f>
+        <v>203.56397567651587</v>
+      </c>
+      <c r="W20" s="32">
+        <f>$C20*(W17/$C17)</f>
+        <v>204.48232198994847</v>
+      </c>
+      <c r="X20" s="32">
+        <f>$C20*(X17/$C17)</f>
+        <v>205.37051374105332</v>
+      </c>
+      <c r="Y20" s="32">
+        <f>$C20*(Y17/$C17)</f>
+        <v>206.23111827310038</v>
+      </c>
+      <c r="Z20" s="32">
+        <f>$C20*(Z17/$C17)</f>
+        <v>207.0663459302514</v>
+      </c>
+      <c r="AA20" s="32">
+        <f>$C20*(AA17/$C17)</f>
+        <v>207.87652772750224</v>
+      </c>
+      <c r="AB20" s="32">
+        <f>$C20*(AB17/$C17)</f>
+        <v>208.66177325002221</v>
+      </c>
+      <c r="AC20" s="32">
+        <f>$C20*(AC17/$C17)</f>
+        <v>209.4242092409161</v>
+      </c>
+      <c r="AD20" s="32">
+        <f>$C20*(AD17/$C17)</f>
+        <v>210.16650133118304</v>
+      </c>
+      <c r="AE20" s="32">
+        <f>$C20*(AE17/$C17)</f>
+        <v>210.89121121537289</v>
+      </c>
+      <c r="AF20" s="32">
+        <f>$C20*(AF17/$C17)</f>
+        <v>211.59996233563251</v>
+      </c>
+      <c r="AG20" s="32">
+        <f>$C20*(AG17/$C17)</f>
+        <v>212.2945097492865</v>
+      </c>
+      <c r="AH20" s="32">
+        <f>$C20*(AH17/$C17)</f>
+        <v>212.97778457717698</v>
+      </c>
+      <c r="AI20" s="32">
+        <f>$C20*(AI17/$C17)</f>
+        <v>213.65305234437406</v>
+      </c>
+      <c r="AJ20" s="32">
+        <f>$C20*(AJ17/$C17)</f>
+        <v>214.32322666068771</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="35">
+        <f>B13</f>
+        <v>78.746413233795309</v>
+      </c>
+      <c r="E21" s="32">
+        <f>$D21*(E17/$D17)</f>
+        <v>79.22035457441639</v>
+      </c>
+      <c r="F21" s="32">
+        <f>$D21*(F17/$D17)</f>
+        <v>79.686851152261795</v>
+      </c>
+      <c r="G21" s="32">
+        <f>$D21*(G17/$D17)</f>
+        <v>80.147256188504812</v>
+      </c>
+      <c r="H21" s="32">
+        <f>$D21*(H17/$D17)</f>
+        <v>80.602308766760771</v>
+      </c>
+      <c r="I21" s="32">
+        <f>$D21*(I17/$D17)</f>
+        <v>81.053453831609303</v>
+      </c>
+      <c r="J21" s="32">
+        <f>$D21*(J17/$D17)</f>
+        <v>81.502039307858951</v>
+      </c>
+      <c r="K21" s="32">
+        <f>$D21*(K17/$D17)</f>
+        <v>81.949110746044468</v>
+      </c>
+      <c r="L21" s="32">
+        <f>$D21*(L17/$D17)</f>
+        <v>82.395057669712912</v>
+      </c>
+      <c r="M21" s="32">
+        <f>$D21*(M17/$D17)</f>
+        <v>82.840126600565355</v>
+      </c>
+      <c r="N21" s="32">
+        <f>$D21*(N17/$D17)</f>
+        <v>83.284816119112293</v>
+      </c>
+      <c r="O21" s="32">
+        <f>$D21*(O17/$D17)</f>
+        <v>83.7295167118763</v>
+      </c>
+      <c r="P21" s="32">
+        <f>$D21*(P17/$D17)</f>
+        <v>84.174130877598614</v>
+      </c>
+      <c r="Q21" s="32">
+        <f>$D21*(Q17/$D17)</f>
+        <v>84.619098214546923</v>
+      </c>
+      <c r="R21" s="32">
+        <f>$D21*(R17/$D17)</f>
+        <v>85.063336579121497</v>
+      </c>
+      <c r="S21" s="32">
+        <f>$D21*(S17/$D17)</f>
+        <v>85.503288258727025</v>
+      </c>
+      <c r="T21" s="32">
+        <f>$D21*(T17/$D17)</f>
+        <v>85.934232266491435</v>
+      </c>
+      <c r="U21" s="32">
+        <f>$D21*(U17/$D17)</f>
+        <v>86.352651094042088</v>
+      </c>
+      <c r="V21" s="32">
+        <f>$D21*(V17/$D17)</f>
+        <v>86.757308521716226</v>
+      </c>
+      <c r="W21" s="32">
+        <f>$D21*(W17/$D17)</f>
+        <v>87.148700241098155</v>
+      </c>
+      <c r="X21" s="32">
+        <f>$D21*(X17/$D17)</f>
+        <v>87.527240331607587</v>
+      </c>
+      <c r="Y21" s="32">
+        <f>$D21*(Y17/$D17)</f>
+        <v>87.894022974036631</v>
+      </c>
+      <c r="Z21" s="32">
+        <f>$D21*(Z17/$D17)</f>
+        <v>88.249990199065039</v>
+      </c>
+      <c r="AA21" s="32">
+        <f>$D21*(AA17/$D17)</f>
+        <v>88.595283082588153</v>
+      </c>
+      <c r="AB21" s="32">
+        <f>$D21*(AB17/$D17)</f>
+        <v>88.929948328912573</v>
+      </c>
+      <c r="AC21" s="32">
+        <f>$D21*(AC17/$D17)</f>
+        <v>89.254892338628494</v>
+      </c>
+      <c r="AD21" s="32">
+        <f>$D21*(AD17/$D17)</f>
+        <v>89.571251181957706</v>
+      </c>
+      <c r="AE21" s="32">
+        <f>$D21*(AE17/$D17)</f>
+        <v>89.880116632253817</v>
+      </c>
+      <c r="AF21" s="32">
+        <f>$D21*(AF17/$D17)</f>
+        <v>90.182180587337868</v>
+      </c>
+      <c r="AG21" s="32">
+        <f>$D21*(AG17/$D17)</f>
+        <v>90.478191038347589</v>
+      </c>
+      <c r="AH21" s="32">
+        <f>$D21*(AH17/$D17)</f>
+        <v>90.769397205113634</v>
+      </c>
+      <c r="AI21" s="32">
+        <f>$D21*(AI17/$D17)</f>
+        <v>91.057190827825067</v>
+      </c>
+      <c r="AJ21" s="32">
+        <f>$D21*(AJ17/$D17)</f>
+        <v>91.342813663253224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="32">
+        <f>SUM(D20:D21)</f>
+        <v>263.51393566246452</v>
+      </c>
+      <c r="E22" s="32">
+        <f t="shared" ref="E22:AJ22" si="0">SUM(E20:E21)</f>
+        <v>265.09991453834567</v>
+      </c>
+      <c r="F22" s="32">
+        <f t="shared" si="0"/>
+        <v>266.66098054951931</v>
+      </c>
+      <c r="G22" s="32">
+        <f t="shared" si="0"/>
+        <v>268.2016620627079</v>
+      </c>
+      <c r="H22" s="32">
+        <f t="shared" si="0"/>
+        <v>269.72443231858682</v>
+      </c>
+      <c r="I22" s="32">
+        <f t="shared" si="0"/>
+        <v>271.2341266235195</v>
+      </c>
+      <c r="J22" s="32">
+        <f t="shared" si="0"/>
+        <v>272.73525562067914</v>
+      </c>
+      <c r="K22" s="32">
+        <f t="shared" si="0"/>
+        <v>274.23131809972529</v>
+      </c>
+      <c r="L22" s="32">
+        <f t="shared" si="0"/>
+        <v>275.72361754711153</v>
+      </c>
+      <c r="M22" s="32">
+        <f t="shared" si="0"/>
+        <v>277.21297891347382</v>
+      </c>
+      <c r="N22" s="32">
+        <f t="shared" si="0"/>
+        <v>278.70107062924814</v>
+      </c>
+      <c r="O22" s="32">
+        <f t="shared" si="0"/>
+        <v>280.18919940335184</v>
+      </c>
+      <c r="P22" s="32">
+        <f t="shared" si="0"/>
+        <v>281.67703896136351</v>
+      </c>
+      <c r="Q22" s="32">
+        <f t="shared" si="0"/>
+        <v>283.16606035783479</v>
+      </c>
+      <c r="R22" s="32">
+        <f t="shared" si="0"/>
+        <v>284.65264234949638</v>
+      </c>
+      <c r="S22" s="32">
+        <f t="shared" si="0"/>
+        <v>286.12487954523965</v>
+      </c>
+      <c r="T22" s="32">
+        <f t="shared" si="0"/>
+        <v>287.56697381814325</v>
+      </c>
+      <c r="U22" s="32">
+        <f t="shared" si="0"/>
+        <v>288.96715431494624</v>
+      </c>
+      <c r="V22" s="32">
+        <f t="shared" si="0"/>
+        <v>290.32128419823209</v>
+      </c>
+      <c r="W22" s="32">
+        <f t="shared" si="0"/>
+        <v>291.63102223104664</v>
+      </c>
+      <c r="X22" s="32">
+        <f t="shared" si="0"/>
+        <v>292.89775407266092</v>
+      </c>
+      <c r="Y22" s="32">
+        <f t="shared" si="0"/>
+        <v>294.12514124713698</v>
+      </c>
+      <c r="Z22" s="32">
+        <f t="shared" si="0"/>
+        <v>295.31633612931643</v>
+      </c>
+      <c r="AA22" s="32">
+        <f t="shared" si="0"/>
+        <v>296.4718108100904</v>
+      </c>
+      <c r="AB22" s="32">
+        <f t="shared" si="0"/>
+        <v>297.59172157893477</v>
+      </c>
+      <c r="AC22" s="32">
+        <f t="shared" si="0"/>
+        <v>298.67910157954458</v>
+      </c>
+      <c r="AD22" s="32">
+        <f t="shared" si="0"/>
+        <v>299.73775251314078</v>
+      </c>
+      <c r="AE22" s="32">
+        <f t="shared" si="0"/>
+        <v>300.77132784762671</v>
+      </c>
+      <c r="AF22" s="32">
+        <f t="shared" si="0"/>
+        <v>301.78214292297037</v>
+      </c>
+      <c r="AG22" s="32">
+        <f t="shared" si="0"/>
+        <v>302.77270078763411</v>
+      </c>
+      <c r="AH22" s="32">
+        <f t="shared" si="0"/>
+        <v>303.74718178229062</v>
+      </c>
+      <c r="AI22" s="32">
+        <f t="shared" si="0"/>
+        <v>304.71024317219911</v>
+      </c>
+      <c r="AJ22" s="32">
+        <f t="shared" si="0"/>
+        <v>305.66604032394093</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -6045,15 +7039,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.59765625" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="B1">
         <v>2018</v>
@@ -6155,7 +7149,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6292,7 +7286,7 @@
         <v>27308360240.000004</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6396,7 +7390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -6533,7 +7527,7 @@
         <v>113879348860.00002</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6670,7 +7664,7 @@
         <v>1954220107240.0002</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -6774,111 +7768,144 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <v>0</v>
-      </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
-      <c r="AG7">
-        <v>0</v>
-      </c>
-      <c r="AH7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="B7" s="26">
+        <f>'water &amp; waste'!D22*10^9</f>
+        <v>263513935662.46451</v>
+      </c>
+      <c r="C7" s="26">
+        <f>'water &amp; waste'!E22*10^9</f>
+        <v>265099914538.34567</v>
+      </c>
+      <c r="D7" s="26">
+        <f>'water &amp; waste'!F22*10^9</f>
+        <v>266660980549.51932</v>
+      </c>
+      <c r="E7" s="26">
+        <f>'water &amp; waste'!G22*10^9</f>
+        <v>268201662062.70789</v>
+      </c>
+      <c r="F7" s="26">
+        <f>'water &amp; waste'!H22*10^9</f>
+        <v>269724432318.58682</v>
+      </c>
+      <c r="G7" s="26">
+        <f>'water &amp; waste'!I22*10^9</f>
+        <v>271234126623.5195</v>
+      </c>
+      <c r="H7" s="26">
+        <f>'water &amp; waste'!J22*10^9</f>
+        <v>272735255620.67914</v>
+      </c>
+      <c r="I7" s="26">
+        <f>'water &amp; waste'!K22*10^9</f>
+        <v>274231318099.72528</v>
+      </c>
+      <c r="J7" s="26">
+        <f>'water &amp; waste'!L22*10^9</f>
+        <v>275723617547.11151</v>
+      </c>
+      <c r="K7" s="26">
+        <f>'water &amp; waste'!M22*10^9</f>
+        <v>277212978913.47382</v>
+      </c>
+      <c r="L7" s="26">
+        <f>'water &amp; waste'!N22*10^9</f>
+        <v>278701070629.24811</v>
+      </c>
+      <c r="M7" s="26">
+        <f>'water &amp; waste'!O22*10^9</f>
+        <v>280189199403.35181</v>
+      </c>
+      <c r="N7" s="26">
+        <f>'water &amp; waste'!P22*10^9</f>
+        <v>281677038961.36353</v>
+      </c>
+      <c r="O7" s="26">
+        <f>'water &amp; waste'!Q22*10^9</f>
+        <v>283166060357.83478</v>
+      </c>
+      <c r="P7" s="26">
+        <f>'water &amp; waste'!R22*10^9</f>
+        <v>284652642349.4964</v>
+      </c>
+      <c r="Q7" s="26">
+        <f>'water &amp; waste'!S22*10^9</f>
+        <v>286124879545.23962</v>
+      </c>
+      <c r="R7" s="26">
+        <f>'water &amp; waste'!T22*10^9</f>
+        <v>287566973818.14325</v>
+      </c>
+      <c r="S7" s="26">
+        <f>'water &amp; waste'!U22*10^9</f>
+        <v>288967154314.94623</v>
+      </c>
+      <c r="T7" s="26">
+        <f>'water &amp; waste'!V22*10^9</f>
+        <v>290321284198.23212</v>
+      </c>
+      <c r="U7" s="26">
+        <f>'water &amp; waste'!W22*10^9</f>
+        <v>291631022231.04663</v>
+      </c>
+      <c r="V7" s="26">
+        <f>'water &amp; waste'!X22*10^9</f>
+        <v>292897754072.66089</v>
+      </c>
+      <c r="W7" s="26">
+        <f>'water &amp; waste'!Y22*10^9</f>
+        <v>294125141247.13696</v>
+      </c>
+      <c r="X7" s="26">
+        <f>'water &amp; waste'!Z22*10^9</f>
+        <v>295316336129.31641</v>
+      </c>
+      <c r="Y7" s="26">
+        <f>'water &amp; waste'!AA22*10^9</f>
+        <v>296471810810.09039</v>
+      </c>
+      <c r="Z7" s="26">
+        <f>'water &amp; waste'!AB22*10^9</f>
+        <v>297591721578.93475</v>
+      </c>
+      <c r="AA7" s="26">
+        <f>'water &amp; waste'!AC22*10^9</f>
+        <v>298679101579.54456</v>
+      </c>
+      <c r="AB7" s="26">
+        <f>'water &amp; waste'!AD22*10^9</f>
+        <v>299737752513.14075</v>
+      </c>
+      <c r="AC7" s="26">
+        <f>'water &amp; waste'!AE22*10^9</f>
+        <v>300771327847.62671</v>
+      </c>
+      <c r="AD7" s="26">
+        <f>'water &amp; waste'!AF22*10^9</f>
+        <v>301782142922.97034</v>
+      </c>
+      <c r="AE7" s="26">
+        <f>'water &amp; waste'!AG22*10^9</f>
+        <v>302772700787.63409</v>
+      </c>
+      <c r="AF7" s="26">
+        <f>'water &amp; waste'!AH22*10^9</f>
+        <v>303747181782.29065</v>
+      </c>
+      <c r="AG7" s="26">
+        <f>'water &amp; waste'!AI22*10^9</f>
+        <v>304710243172.1991</v>
+      </c>
+      <c r="AH7" s="26">
+        <f>'water &amp; waste'!AJ22*10^9</f>
+        <v>305666040323.94092</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -7015,7 +8042,7 @@
         <v>564062085960.00012</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -7152,7 +8179,7 @@
         <v>8157743515200</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
     </row>
   </sheetData>

</xml_diff>